<commit_message>
Checking in report progress.
</commit_message>
<xml_diff>
--- a/TestResults_Data.xlsx
+++ b/TestResults_Data.xlsx
@@ -107,31 +107,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Average</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -165,14 +140,25 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg Running Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -183,7 +169,37 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:val>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$L$3:$L$9</c:f>
               <c:numCache>
@@ -212,7 +228,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
@@ -223,17 +239,31 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="476449672"/>
-        <c:axId val="476453200"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="476449672"/>
+        <c:axId val="477359552"/>
+        <c:axId val="477359944"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="477359552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -242,8 +272,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -270,15 +300,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="476453200"/>
+        <c:crossAx val="477359944"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="476453200"/>
+        <c:axId val="477359944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -304,8 +331,14 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -329,9 +362,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="476449672"/>
+        <c:crossAx val="477359552"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -393,31 +426,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Min</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -451,14 +459,25 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Min Running Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -469,7 +488,37 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:val>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$M$3:$M$9</c:f>
               <c:numCache>
@@ -498,7 +547,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
@@ -509,17 +558,31 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="476446536"/>
-        <c:axId val="476447712"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="476446536"/>
+        <c:axId val="511138896"/>
+        <c:axId val="511136544"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="511138896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -528,8 +591,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -556,15 +619,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="476447712"/>
+        <c:crossAx val="511136544"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="476447712"/>
+        <c:axId val="511136544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -590,8 +650,14 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -615,9 +681,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="476446536"/>
+        <c:crossAx val="511138896"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -679,31 +745,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Max</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -737,14 +778,25 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Max Running Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -755,7 +807,37 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:val>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$N$3:$N$9</c:f>
               <c:numCache>
@@ -784,7 +866,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
@@ -795,17 +877,31 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="515060888"/>
-        <c:axId val="515065984"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="515060888"/>
+        <c:axId val="511140464"/>
+        <c:axId val="511137328"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="511140464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -814,8 +910,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -842,15 +938,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="515065984"/>
+        <c:crossAx val="511137328"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="515065984"/>
+        <c:axId val="511137328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -876,8 +969,14 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -901,9 +1000,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="515060888"/>
+        <c:crossAx val="511140464"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1071,7 +1170,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1098,8 +1197,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1179,11 +1278,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -1194,11 +1288,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -1210,7 +1299,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1230,9 +1319,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1245,10 +1331,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1288,22 +1374,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1408,8 +1495,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1541,19 +1628,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1567,6 +1655,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1587,7 +1686,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1614,8 +1713,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1695,11 +1794,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -1710,11 +1804,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -1726,7 +1815,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1746,9 +1835,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1761,10 +1847,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1804,22 +1890,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1924,8 +2011,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2057,19 +2144,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2083,6 +2171,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -2103,7 +2202,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2130,8 +2229,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2211,11 +2310,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -2226,11 +2320,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -2242,7 +2331,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2262,9 +2351,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2277,10 +2363,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2320,22 +2406,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -2440,8 +2527,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2573,19 +2660,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2599,6 +2687,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -2623,19 +2722,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>61232</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>2722</xdr:rowOff>
+      <xdr:colOff>503465</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>29936</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>748393</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>27213</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>176893</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>106136</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2653,19 +2752,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>102052</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>16328</xdr:rowOff>
+      <xdr:colOff>517072</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>70757</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>748392</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>40821</xdr:rowOff>
+      <xdr:rowOff>146957</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2683,19 +2782,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>74837</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>138793</xdr:rowOff>
+      <xdr:colOff>462643</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>179615</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>857249</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>54429</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>136071</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>65315</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3002,8 +3101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M42" sqref="M42:N42"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M13" sqref="C13:M58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3098,15 +3197,15 @@
         <v>14972</v>
       </c>
       <c r="L3">
-        <f>AVERAGE(B3:K3)</f>
+        <f t="shared" ref="L3:L9" si="0">AVERAGE(B3:K3)</f>
         <v>14964.6</v>
       </c>
       <c r="M3">
-        <f>MIN(B3:K3)</f>
+        <f t="shared" ref="M3:M9" si="1">MIN(B3:K3)</f>
         <v>13780</v>
       </c>
       <c r="N3">
-        <f>MAX(B3:K3)</f>
+        <f t="shared" ref="N3:N9" si="2">MAX(B3:K3)</f>
         <v>16589</v>
       </c>
     </row>
@@ -3145,15 +3244,15 @@
         <v>16697</v>
       </c>
       <c r="L4">
-        <f>AVERAGE(B4:K4)</f>
+        <f t="shared" si="0"/>
         <v>15269</v>
       </c>
       <c r="M4">
-        <f>MIN(B4:K4)</f>
+        <f t="shared" si="1"/>
         <v>14607</v>
       </c>
       <c r="N4">
-        <f>MAX(B4:K4)</f>
+        <f t="shared" si="2"/>
         <v>16697</v>
       </c>
     </row>
@@ -3192,15 +3291,15 @@
         <v>14788</v>
       </c>
       <c r="L5">
-        <f>AVERAGE(B5:K5)</f>
+        <f t="shared" si="0"/>
         <v>15010.9</v>
       </c>
       <c r="M5">
-        <f>MIN(B5:K5)</f>
+        <f t="shared" si="1"/>
         <v>13727</v>
       </c>
       <c r="N5">
-        <f>MAX(B5:K5)</f>
+        <f t="shared" si="2"/>
         <v>15885</v>
       </c>
     </row>
@@ -3239,15 +3338,15 @@
         <v>15219</v>
       </c>
       <c r="L6">
-        <f>AVERAGE(B6:K6)</f>
+        <f t="shared" si="0"/>
         <v>15048.6</v>
       </c>
       <c r="M6">
-        <f>MIN(B6:K6)</f>
+        <f t="shared" si="1"/>
         <v>14733</v>
       </c>
       <c r="N6">
-        <f>MAX(B6:K6)</f>
+        <f t="shared" si="2"/>
         <v>16003</v>
       </c>
     </row>
@@ -3286,15 +3385,15 @@
         <v>14687</v>
       </c>
       <c r="L7">
-        <f>AVERAGE(B7:K7)</f>
+        <f t="shared" si="0"/>
         <v>15065.6</v>
       </c>
       <c r="M7">
-        <f>MIN(B7:K7)</f>
+        <f t="shared" si="1"/>
         <v>14687</v>
       </c>
       <c r="N7">
-        <f>MAX(B7:K7)</f>
+        <f t="shared" si="2"/>
         <v>15830</v>
       </c>
     </row>
@@ -3333,15 +3432,15 @@
         <v>15666</v>
       </c>
       <c r="L8">
-        <f>AVERAGE(B8:K8)</f>
+        <f t="shared" si="0"/>
         <v>14990.5</v>
       </c>
       <c r="M8">
-        <f>MIN(B8:K8)</f>
+        <f t="shared" si="1"/>
         <v>14711</v>
       </c>
       <c r="N8">
-        <f>MAX(B8:K8)</f>
+        <f t="shared" si="2"/>
         <v>15779</v>
       </c>
     </row>
@@ -3380,15 +3479,15 @@
         <v>14825</v>
       </c>
       <c r="L9">
-        <f>AVERAGE(B9:K9)</f>
+        <f t="shared" si="0"/>
         <v>15222.5</v>
       </c>
       <c r="M9">
-        <f>MIN(B9:K9)</f>
+        <f t="shared" si="1"/>
         <v>14719</v>
       </c>
       <c r="N9">
-        <f>MAX(B9:K9)</f>
+        <f t="shared" si="2"/>
         <v>15865</v>
       </c>
     </row>

</xml_diff>